<commit_message>
- Sonderzeichen entfernt - XPathes aktualisiert - Fehler im CSV Export behoben -
</commit_message>
<xml_diff>
--- a/Datentreiber.xlsx
+++ b/Datentreiber.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnaas\IdeaProjects\SeleniumTestobject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnaas\IdeaProjects\VakanzenGrabber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC464FEC-936B-437C-B2A3-29A1A259F8FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C26449-8356-4B27-B04A-6970BEEDFAAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23070" yWindow="2835" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testdaten" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>URL</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t>Testanalyst</t>
-  </si>
-  <si>
-    <t>Testautomatisierer</t>
-  </si>
-  <si>
-    <t>Testmanager</t>
   </si>
   <si>
     <t>FreelanceDE</t>
@@ -885,7 +879,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,27 +898,17 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- config.xml - FreelanceMap ergänz - Test.java - FreelanceMap in Switch-Case ergänzt - VakanzenGrabber.webelementFinden - Linktext identifikation ergänzt - Testdatum.eSeite - Identifikation Freelancermap ergänzt
</commit_message>
<xml_diff>
--- a/Datentreiber.xlsx
+++ b/Datentreiber.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnaas\IdeaProjects\VakanzenGrabber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C26449-8356-4B27-B04A-6970BEEDFAAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A818FFD-3E9D-4FE7-A341-E4D0B549F494}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testdaten" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>URL</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>FreelanceDE</t>
+  </si>
+  <si>
+    <t>FreelancerMap</t>
+  </si>
+  <si>
+    <t>Testmanager</t>
   </si>
 </sst>
 </file>
@@ -876,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,20 +904,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Package - FreelancerMap ergänzt
</commit_message>
<xml_diff>
--- a/Datentreiber.xlsx
+++ b/Datentreiber.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnaas\IdeaProjects\VakanzenGrabber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A818FFD-3E9D-4FE7-A341-E4D0B549F494}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8073E426-0ADF-4947-BB0D-31EE09D60300}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testdaten" sheetId="1" r:id="rId1"/>
@@ -23,21 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>URL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Suchbegriff</t>
   </si>
   <si>
     <t>Testanalyst</t>
-  </si>
-  <si>
-    <t>FreelanceDE</t>
-  </si>
-  <si>
-    <t>FreelancerMap</t>
   </si>
   <si>
     <t>Testmanager</t>
@@ -524,9 +515,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -882,40 +872,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Package - ExtendetLogger changed - Changed Logger to ExtendedReports
</commit_message>
<xml_diff>
--- a/Datentreiber.xlsx
+++ b/Datentreiber.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnaas\IdeaProjects\VakanzenGrabber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8073E426-0ADF-4947-BB0D-31EE09D60300}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B90503-F748-4AC3-97CA-CA314CA963F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testdaten" sheetId="1" r:id="rId1"/>
@@ -23,15 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Suchbegriff</t>
   </si>
   <si>
     <t>Testanalyst</t>
-  </si>
-  <si>
-    <t>Testmanager</t>
   </si>
 </sst>
 </file>
@@ -872,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -890,11 +887,6 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>